<commit_message>
Final Version: Before the last interview
</commit_message>
<xml_diff>
--- a/samples/attendance_sample.xlsx
+++ b/samples/attendance_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lokesh Vyas\Downloads\New folder\leave-productivity-analyzer\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\leave-productivity-analyzer\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CBABF0-91FF-4A29-BEA6-C0E91B41D3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C12F044-7555-46D7-B406-CF94F1E11166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>